<commit_message>
minor changes in manual csv file
</commit_message>
<xml_diff>
--- a/collect_organisations/manual/uni-potsdam-repo.xlsx
+++ b/collect_organisations/manual/uni-potsdam-repo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devkate/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/devkate/Downloads/Thesis/SWORDS-UP/collect_organisations/manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DE8001-C6DA-8C4B-B39C-F13CE7C52A67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CCBF54-D2AA-414F-BF27-DFE5D5E743AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1000" yWindow="500" windowWidth="50200" windowHeight="26700" xr2:uid="{6D7B27A1-11D9-9E40-88B4-404111C7F8FF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="199">
   <si>
     <t xml:space="preserve">Organisation </t>
   </si>
@@ -625,6 +625,27 @@
   </si>
   <si>
     <t>Potsdam ACM</t>
+  </si>
+  <si>
+    <t>FAIR-Test-All</t>
+  </si>
+  <si>
+    <t>https://github.com/SemanticM+B9+B10+B11+B+B23</t>
+  </si>
+  <si>
+    <t>Included or Not</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>=</t>
   </si>
 </sst>
 </file>
@@ -1051,10 +1072,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95E93D60-4FE4-A942-A3FA-89441F0ED0E5}">
-  <dimension ref="A1:K126"/>
+  <dimension ref="A1:P126"/>
   <sheetViews>
     <sheetView tabSelected="1" showWhiteSpace="0" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1064,7 +1085,7 @@
     <col min="3" max="3" width="73.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1086,11 +1107,17 @@
       <c r="I1" t="s">
         <v>40</v>
       </c>
+      <c r="J1" t="s">
+        <v>192</v>
+      </c>
       <c r="K1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="M1" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -1112,8 +1139,11 @@
       <c r="K2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1135,8 +1165,11 @@
       <c r="K3" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1158,8 +1191,11 @@
       <c r="K4" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M4" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1181,8 +1217,11 @@
       <c r="K5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M5" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>16</v>
       </c>
@@ -1204,8 +1243,11 @@
       <c r="K6" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="M6" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1227,13 +1269,16 @@
       <c r="K7" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M7" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>20</v>
+        <v>193</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -1250,8 +1295,11 @@
       <c r="K8" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>24</v>
       </c>
@@ -1270,8 +1318,11 @@
       <c r="K9" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M9" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1287,8 +1338,11 @@
       <c r="K10" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M10" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -1310,8 +1364,11 @@
       <c r="K11" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="M11" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -1333,8 +1390,11 @@
       <c r="K12" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="18" x14ac:dyDescent="0.2">
+      <c r="M12" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -1356,8 +1416,11 @@
       <c r="K13" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="M13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>46</v>
       </c>
@@ -1371,7 +1434,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>48</v>
       </c>
@@ -1387,7 +1450,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>50</v>
       </c>
@@ -1403,7 +1466,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="9" t="s">
         <v>52</v>
       </c>
@@ -1419,7 +1482,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>54</v>
       </c>
@@ -1435,7 +1498,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="10" t="s">
         <v>57</v>
@@ -1447,7 +1510,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>59</v>
       </c>
@@ -1463,11 +1526,11 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B24" s="1" t="s">
         <v>61</v>
       </c>
       <c r="C24" s="11" t="s">
@@ -1479,7 +1542,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>65</v>
       </c>
@@ -1495,7 +1558,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" ht="34" x14ac:dyDescent="0.2">
       <c r="A26" s="9" t="s">
         <v>68</v>
       </c>
@@ -1509,7 +1572,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>70</v>
       </c>
@@ -1524,12 +1587,15 @@
       <c r="K27" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="P27" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B28" s="11" t="s">
+      <c r="B28" s="1" t="s">
         <v>72</v>
       </c>
       <c r="C28" s="11" t="s">
@@ -1541,7 +1607,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>74</v>
       </c>
@@ -1551,11 +1617,17 @@
       <c r="C29" s="11"/>
       <c r="D29" s="11"/>
       <c r="E29" s="11"/>
+      <c r="J29" t="s">
+        <v>196</v>
+      </c>
       <c r="K29" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M29" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>75</v>
       </c>
@@ -1571,7 +1643,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>78</v>
       </c>
@@ -1587,7 +1659,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>81</v>
       </c>
@@ -1601,7 +1673,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>83</v>
       </c>
@@ -1617,7 +1689,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>87</v>
       </c>
@@ -1629,11 +1701,17 @@
       </c>
       <c r="D34" s="11"/>
       <c r="E34" s="11"/>
+      <c r="J34" t="s">
+        <v>196</v>
+      </c>
       <c r="K34" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M34" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>89</v>
       </c>
@@ -1647,7 +1725,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>91</v>
       </c>
@@ -1663,7 +1741,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>93</v>
       </c>
@@ -1682,7 +1760,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>95</v>
       </c>
@@ -1694,11 +1772,17 @@
       </c>
       <c r="D38" s="11"/>
       <c r="E38" s="11"/>
+      <c r="J38" t="s">
+        <v>197</v>
+      </c>
       <c r="K38" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M38" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>98</v>
       </c>
@@ -1714,7 +1798,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>101</v>
       </c>
@@ -1724,11 +1808,17 @@
       <c r="C40" s="11"/>
       <c r="D40" s="11"/>
       <c r="E40" s="11"/>
+      <c r="J40" t="s">
+        <v>197</v>
+      </c>
       <c r="K40" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M40" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>103</v>
       </c>
@@ -1740,11 +1830,17 @@
       </c>
       <c r="D41" s="11"/>
       <c r="E41" s="11"/>
+      <c r="J41" t="s">
+        <v>197</v>
+      </c>
       <c r="K41" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="M41" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>106</v>
       </c>
@@ -1758,7 +1854,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>108</v>
       </c>
@@ -1772,7 +1868,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="9" t="s">
         <v>110</v>
       </c>
@@ -1786,7 +1882,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>112</v>
       </c>
@@ -1800,7 +1896,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
       <c r="B46" s="10" t="s">
         <v>114</v>
@@ -1812,7 +1908,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>183</v>
       </c>
@@ -1828,7 +1924,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
       <c r="B48" s="10" t="s">
         <v>47</v>
@@ -2780,6 +2876,8 @@
     <hyperlink ref="B85" r:id="rId101" xr:uid="{62EBCF91-DE9F-8E46-9519-353B10380B61}"/>
     <hyperlink ref="B86" r:id="rId102" xr:uid="{60853555-EC35-7143-89CA-EFB3337A2E7E}"/>
     <hyperlink ref="B87" r:id="rId103" xr:uid="{80581A85-B75D-6E4F-8EE4-26D314B43C2A}"/>
+    <hyperlink ref="B24" r:id="rId104" xr:uid="{5E8BA66B-B04C-0C45-9821-21CD324A5D94}"/>
+    <hyperlink ref="B28" r:id="rId105" xr:uid="{F17D73FA-D242-D244-AB89-9A8A1C17F554}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>